<commit_message>
Fix minor bugs page analytics
</commit_message>
<xml_diff>
--- a/input/bang_cuoc_phi.xlsx
+++ b/input/bang_cuoc_phi.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SUPERAI\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/trinhlk2/Desktop/superai/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1ECB3900-6E82-4ABB-B3CA-907A5689184C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED06FD6C-E133-1641-A7A8-7A20ED63A23F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26205" yWindow="0" windowWidth="24765" windowHeight="14790" xr2:uid="{5D136356-3F40-4A14-B42C-374F0CC1DB9E}"/>
+    <workbookView xWindow="4440" yWindow="760" windowWidth="21360" windowHeight="18880" xr2:uid="{5D136356-3F40-4A14-B42C-374F0CC1DB9E}"/>
   </bookViews>
   <sheets>
     <sheet name="Bảng Giá Khối Lượng" sheetId="4" r:id="rId1"/>
@@ -934,7 +934,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="121">
+  <cellXfs count="122">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1108,96 +1108,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="40" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
@@ -1249,9 +1159,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1287,6 +1194,102 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1611,155 +1614,155 @@
   <dimension ref="A1:CA169"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C93" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="AB3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="O8" sqref="O8"/>
+      <selection pane="bottomRight" activeCell="AN14" sqref="AN14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5" customWidth="1"/>
+    <col min="2" max="2" width="9.5" bestFit="1" customWidth="1"/>
     <col min="3" max="13" width="8" style="1" customWidth="1"/>
-    <col min="37" max="37" width="10.7109375" customWidth="1"/>
+    <col min="37" max="37" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:79" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="83" t="s">
+    <row r="1" spans="1:79" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="114" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="84"/>
-      <c r="C1" s="88" t="s">
+      <c r="B1" s="115"/>
+      <c r="C1" s="119" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="89"/>
-      <c r="E1" s="89"/>
-      <c r="F1" s="89"/>
-      <c r="G1" s="89"/>
-      <c r="H1" s="89"/>
-      <c r="I1" s="89"/>
-      <c r="J1" s="89"/>
-      <c r="K1" s="89"/>
-      <c r="L1" s="89"/>
-      <c r="M1" s="90"/>
-      <c r="N1" s="85" t="s">
+      <c r="D1" s="120"/>
+      <c r="E1" s="120"/>
+      <c r="F1" s="120"/>
+      <c r="G1" s="120"/>
+      <c r="H1" s="120"/>
+      <c r="I1" s="120"/>
+      <c r="J1" s="120"/>
+      <c r="K1" s="120"/>
+      <c r="L1" s="120"/>
+      <c r="M1" s="121"/>
+      <c r="N1" s="116" t="s">
         <v>1</v>
       </c>
-      <c r="O1" s="86"/>
-      <c r="P1" s="86"/>
-      <c r="Q1" s="86"/>
-      <c r="R1" s="86"/>
-      <c r="S1" s="86"/>
-      <c r="T1" s="86"/>
-      <c r="U1" s="86"/>
-      <c r="V1" s="86"/>
-      <c r="W1" s="86"/>
-      <c r="X1" s="87"/>
-      <c r="Y1" s="80" t="s">
+      <c r="O1" s="117"/>
+      <c r="P1" s="117"/>
+      <c r="Q1" s="117"/>
+      <c r="R1" s="117"/>
+      <c r="S1" s="117"/>
+      <c r="T1" s="117"/>
+      <c r="U1" s="117"/>
+      <c r="V1" s="117"/>
+      <c r="W1" s="117"/>
+      <c r="X1" s="118"/>
+      <c r="Y1" s="111" t="s">
         <v>11</v>
       </c>
-      <c r="Z1" s="81"/>
-      <c r="AA1" s="81"/>
-      <c r="AB1" s="81"/>
-      <c r="AC1" s="81"/>
-      <c r="AD1" s="81"/>
-      <c r="AE1" s="81"/>
-      <c r="AF1" s="81"/>
-      <c r="AG1" s="81"/>
-      <c r="AH1" s="81"/>
-      <c r="AI1" s="82"/>
-      <c r="AJ1" s="77" t="s">
+      <c r="Z1" s="112"/>
+      <c r="AA1" s="112"/>
+      <c r="AB1" s="112"/>
+      <c r="AC1" s="112"/>
+      <c r="AD1" s="112"/>
+      <c r="AE1" s="112"/>
+      <c r="AF1" s="112"/>
+      <c r="AG1" s="112"/>
+      <c r="AH1" s="112"/>
+      <c r="AI1" s="113"/>
+      <c r="AJ1" s="108" t="s">
         <v>2</v>
       </c>
-      <c r="AK1" s="78"/>
-      <c r="AL1" s="78"/>
-      <c r="AM1" s="78"/>
-      <c r="AN1" s="78"/>
-      <c r="AO1" s="78"/>
-      <c r="AP1" s="78"/>
-      <c r="AQ1" s="78"/>
-      <c r="AR1" s="78"/>
-      <c r="AS1" s="78"/>
-      <c r="AT1" s="79"/>
-      <c r="AU1" s="94" t="s">
+      <c r="AK1" s="109"/>
+      <c r="AL1" s="109"/>
+      <c r="AM1" s="109"/>
+      <c r="AN1" s="109"/>
+      <c r="AO1" s="109"/>
+      <c r="AP1" s="109"/>
+      <c r="AQ1" s="109"/>
+      <c r="AR1" s="109"/>
+      <c r="AS1" s="109"/>
+      <c r="AT1" s="110"/>
+      <c r="AU1" s="64" t="s">
         <v>14</v>
       </c>
-      <c r="AV1" s="95"/>
-      <c r="AW1" s="95"/>
-      <c r="AX1" s="95"/>
-      <c r="AY1" s="95"/>
-      <c r="AZ1" s="95"/>
-      <c r="BA1" s="95"/>
-      <c r="BB1" s="95"/>
-      <c r="BC1" s="95"/>
-      <c r="BD1" s="95"/>
-      <c r="BE1" s="95"/>
-      <c r="BF1" s="76" t="s">
+      <c r="AV1" s="65"/>
+      <c r="AW1" s="65"/>
+      <c r="AX1" s="65"/>
+      <c r="AY1" s="65"/>
+      <c r="AZ1" s="65"/>
+      <c r="BA1" s="65"/>
+      <c r="BB1" s="65"/>
+      <c r="BC1" s="65"/>
+      <c r="BD1" s="65"/>
+      <c r="BE1" s="65"/>
+      <c r="BF1" s="96" t="s">
         <v>15</v>
       </c>
-      <c r="BG1" s="76"/>
-      <c r="BH1" s="76"/>
-      <c r="BI1" s="76"/>
-      <c r="BJ1" s="76"/>
-      <c r="BK1" s="76"/>
-      <c r="BL1" s="76"/>
-      <c r="BM1" s="76"/>
-      <c r="BN1" s="76"/>
-      <c r="BO1" s="76"/>
-      <c r="BP1" s="76"/>
-      <c r="BQ1" s="75" t="s">
+      <c r="BG1" s="96"/>
+      <c r="BH1" s="96"/>
+      <c r="BI1" s="96"/>
+      <c r="BJ1" s="96"/>
+      <c r="BK1" s="96"/>
+      <c r="BL1" s="96"/>
+      <c r="BM1" s="96"/>
+      <c r="BN1" s="96"/>
+      <c r="BO1" s="96"/>
+      <c r="BP1" s="96"/>
+      <c r="BQ1" s="95" t="s">
         <v>24</v>
       </c>
-      <c r="BR1" s="75"/>
-      <c r="BS1" s="75"/>
-      <c r="BT1" s="75"/>
-      <c r="BU1" s="75"/>
-      <c r="BV1" s="75"/>
-      <c r="BW1" s="75"/>
-      <c r="BX1" s="75"/>
-      <c r="BY1" s="75"/>
-      <c r="BZ1" s="75"/>
-      <c r="CA1" s="75"/>
+      <c r="BR1" s="95"/>
+      <c r="BS1" s="95"/>
+      <c r="BT1" s="95"/>
+      <c r="BU1" s="95"/>
+      <c r="BV1" s="95"/>
+      <c r="BW1" s="95"/>
+      <c r="BX1" s="95"/>
+      <c r="BY1" s="95"/>
+      <c r="BZ1" s="95"/>
+      <c r="CA1" s="95"/>
     </row>
-    <row r="2" spans="1:79" ht="68.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:79" ht="68.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>16</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="98" t="s">
+      <c r="C2" s="68" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="99" t="s">
+      <c r="D2" s="69" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="100" t="s">
+      <c r="E2" s="70" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="99" t="s">
+      <c r="F2" s="69" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="100" t="s">
+      <c r="G2" s="70" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="100" t="s">
+      <c r="H2" s="70" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="100" t="s">
+      <c r="I2" s="70" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="100" t="s">
+      <c r="J2" s="70" t="s">
         <v>21</v>
       </c>
-      <c r="K2" s="100" t="s">
+      <c r="K2" s="70" t="s">
         <v>22</v>
       </c>
-      <c r="L2" s="100" t="s">
+      <c r="L2" s="70" t="s">
         <v>23</v>
       </c>
-      <c r="M2" s="101" t="s">
+      <c r="M2" s="71" t="s">
         <v>25</v>
       </c>
       <c r="N2" s="10" t="s">
@@ -1828,37 +1831,37 @@
       <c r="AI2" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="AJ2" s="98" t="s">
+      <c r="AJ2" s="68" t="s">
         <v>6</v>
       </c>
-      <c r="AK2" s="99" t="s">
+      <c r="AK2" s="69" t="s">
         <v>7</v>
       </c>
-      <c r="AL2" s="100" t="s">
+      <c r="AL2" s="70" t="s">
         <v>8</v>
       </c>
-      <c r="AM2" s="99" t="s">
+      <c r="AM2" s="69" t="s">
         <v>9</v>
       </c>
-      <c r="AN2" s="100" t="s">
+      <c r="AN2" s="70" t="s">
         <v>3</v>
       </c>
-      <c r="AO2" s="100" t="s">
+      <c r="AO2" s="70" t="s">
         <v>4</v>
       </c>
-      <c r="AP2" s="100" t="s">
+      <c r="AP2" s="70" t="s">
         <v>5</v>
       </c>
-      <c r="AQ2" s="100" t="s">
+      <c r="AQ2" s="70" t="s">
         <v>21</v>
       </c>
-      <c r="AR2" s="100" t="s">
+      <c r="AR2" s="70" t="s">
         <v>22</v>
       </c>
-      <c r="AS2" s="100" t="s">
+      <c r="AS2" s="70" t="s">
         <v>23</v>
       </c>
-      <c r="AT2" s="101" t="s">
+      <c r="AT2" s="71" t="s">
         <v>25</v>
       </c>
       <c r="AU2" s="10" t="s">
@@ -1961,47 +1964,47 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:79" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>0</v>
       </c>
       <c r="B3">
         <v>500</v>
       </c>
-      <c r="C3" s="113">
+      <c r="C3" s="82">
         <v>12</v>
       </c>
-      <c r="D3" s="114">
+      <c r="D3" s="83">
         <v>12</v>
       </c>
-      <c r="E3" s="114">
+      <c r="E3" s="83">
         <v>12</v>
       </c>
-      <c r="F3" s="114">
+      <c r="F3" s="83">
         <v>12</v>
       </c>
-      <c r="G3" s="114">
+      <c r="G3" s="83">
         <v>12</v>
       </c>
-      <c r="H3" s="114">
+      <c r="H3" s="83">
         <v>12</v>
       </c>
-      <c r="I3" s="114">
+      <c r="I3" s="83">
         <v>12</v>
       </c>
-      <c r="J3" s="114">
+      <c r="J3" s="83">
         <v>12</v>
       </c>
-      <c r="K3" s="114">
+      <c r="K3" s="83">
         <v>12</v>
       </c>
-      <c r="L3" s="114">
+      <c r="L3" s="83">
         <v>12</v>
       </c>
-      <c r="M3" s="115">
+      <c r="M3" s="84">
         <v>12</v>
       </c>
-      <c r="N3" s="96">
+      <c r="N3" s="66">
         <v>14</v>
       </c>
       <c r="O3" s="18">
@@ -2064,43 +2067,43 @@
       <c r="AH3" s="18">
         <v>12</v>
       </c>
-      <c r="AI3" s="93">
+      <c r="AI3" s="63">
         <v>12</v>
       </c>
-      <c r="AJ3" s="102">
+      <c r="AJ3" s="72">
         <v>15.5</v>
       </c>
-      <c r="AK3" s="103">
+      <c r="AK3" s="90">
         <v>18</v>
       </c>
-      <c r="AL3" s="103">
+      <c r="AL3" s="73">
         <v>15.5</v>
       </c>
-      <c r="AM3" s="103">
-        <v>17</v>
-      </c>
-      <c r="AN3" s="103">
+      <c r="AM3" s="90">
         <v>18</v>
       </c>
-      <c r="AO3" s="103">
+      <c r="AN3" s="73">
         <v>18</v>
       </c>
-      <c r="AP3" s="103">
+      <c r="AO3" s="73">
         <v>18</v>
       </c>
-      <c r="AQ3" s="103">
+      <c r="AP3" s="73">
         <v>18</v>
       </c>
-      <c r="AR3" s="103">
+      <c r="AQ3" s="73">
         <v>18</v>
       </c>
-      <c r="AS3" s="103">
+      <c r="AR3" s="73">
         <v>18</v>
       </c>
-      <c r="AT3" s="104">
+      <c r="AS3" s="73">
         <v>18</v>
       </c>
-      <c r="AU3" s="96">
+      <c r="AT3" s="74">
+        <v>18</v>
+      </c>
+      <c r="AU3" s="66">
         <v>12</v>
       </c>
       <c r="AV3" s="18">
@@ -2200,7 +2203,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:79" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <f>B3</f>
         <v>500</v>
@@ -2209,7 +2212,7 @@
         <f>B3+500</f>
         <v>1000</v>
       </c>
-      <c r="C4" s="116">
+      <c r="C4" s="85">
         <v>13.5</v>
       </c>
       <c r="D4" s="20">
@@ -2239,7 +2242,7 @@
       <c r="L4" s="20">
         <v>13.5</v>
       </c>
-      <c r="M4" s="117">
+      <c r="M4" s="86">
         <v>13.5</v>
       </c>
       <c r="N4" s="56">
@@ -2305,20 +2308,20 @@
       <c r="AH4" s="20">
         <v>13</v>
       </c>
-      <c r="AI4" s="91">
+      <c r="AI4" s="61">
         <v>13</v>
       </c>
-      <c r="AJ4" s="105">
+      <c r="AJ4" s="75">
         <v>15.5</v>
       </c>
-      <c r="AK4" s="21">
+      <c r="AK4" s="91">
         <v>18</v>
       </c>
       <c r="AL4" s="21">
         <v>15.5</v>
       </c>
-      <c r="AM4" s="21">
-        <v>17</v>
+      <c r="AM4" s="91">
+        <v>18</v>
       </c>
       <c r="AN4" s="21">
         <v>18</v>
@@ -2338,7 +2341,7 @@
       <c r="AS4" s="21">
         <v>18</v>
       </c>
-      <c r="AT4" s="106">
+      <c r="AT4" s="76">
         <v>18</v>
       </c>
       <c r="AU4" s="56">
@@ -2441,7 +2444,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:79" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <f t="shared" ref="A5:A21" si="0">B4</f>
         <v>1000</v>
@@ -2450,7 +2453,7 @@
         <f t="shared" ref="B5:B21" si="1">B4+500</f>
         <v>1500</v>
       </c>
-      <c r="C5" s="116">
+      <c r="C5" s="85">
         <v>13.5</v>
       </c>
       <c r="D5" s="20">
@@ -2480,7 +2483,7 @@
       <c r="L5" s="20">
         <v>13.5</v>
       </c>
-      <c r="M5" s="117">
+      <c r="M5" s="86">
         <v>13.5</v>
       </c>
       <c r="N5" s="56">
@@ -2546,20 +2549,20 @@
       <c r="AH5" s="20">
         <v>16</v>
       </c>
-      <c r="AI5" s="91">
+      <c r="AI5" s="61">
         <v>16</v>
       </c>
-      <c r="AJ5" s="105">
+      <c r="AJ5" s="75">
         <v>15.5</v>
       </c>
-      <c r="AK5" s="21">
+      <c r="AK5" s="91">
         <v>18</v>
       </c>
       <c r="AL5" s="21">
         <v>15.5</v>
       </c>
-      <c r="AM5" s="21">
-        <v>17</v>
+      <c r="AM5" s="91">
+        <v>18</v>
       </c>
       <c r="AN5" s="21">
         <v>18</v>
@@ -2579,7 +2582,7 @@
       <c r="AS5" s="21">
         <v>18</v>
       </c>
-      <c r="AT5" s="106">
+      <c r="AT5" s="76">
         <v>18</v>
       </c>
       <c r="AU5" s="56">
@@ -2682,7 +2685,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:79" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <f t="shared" si="0"/>
         <v>1500</v>
@@ -2691,7 +2694,7 @@
         <f t="shared" si="1"/>
         <v>2000</v>
       </c>
-      <c r="C6" s="116">
+      <c r="C6" s="85">
         <v>13.5</v>
       </c>
       <c r="D6" s="20">
@@ -2721,7 +2724,7 @@
       <c r="L6" s="20">
         <v>13.5</v>
       </c>
-      <c r="M6" s="117">
+      <c r="M6" s="86">
         <v>13.5</v>
       </c>
       <c r="N6" s="56">
@@ -2787,20 +2790,20 @@
       <c r="AH6" s="20">
         <v>16</v>
       </c>
-      <c r="AI6" s="91">
+      <c r="AI6" s="61">
         <v>16</v>
       </c>
-      <c r="AJ6" s="105">
+      <c r="AJ6" s="75">
         <v>15.5</v>
       </c>
-      <c r="AK6" s="21">
+      <c r="AK6" s="91">
         <v>18</v>
       </c>
       <c r="AL6" s="21">
         <v>15.5</v>
       </c>
-      <c r="AM6" s="21">
-        <v>17</v>
+      <c r="AM6" s="91">
+        <v>18</v>
       </c>
       <c r="AN6" s="21">
         <v>18</v>
@@ -2820,7 +2823,7 @@
       <c r="AS6" s="21">
         <v>18</v>
       </c>
-      <c r="AT6" s="106">
+      <c r="AT6" s="76">
         <v>18</v>
       </c>
       <c r="AU6" s="56">
@@ -2923,7 +2926,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:79" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <f t="shared" si="0"/>
         <v>2000</v>
@@ -2932,7 +2935,7 @@
         <f t="shared" si="1"/>
         <v>2500</v>
       </c>
-      <c r="C7" s="116">
+      <c r="C7" s="85">
         <v>18.5</v>
       </c>
       <c r="D7" s="20">
@@ -2962,7 +2965,7 @@
       <c r="L7" s="20">
         <v>28.5</v>
       </c>
-      <c r="M7" s="117">
+      <c r="M7" s="86">
         <v>28.5</v>
       </c>
       <c r="N7" s="56">
@@ -3028,10 +3031,10 @@
       <c r="AH7" s="20">
         <v>26</v>
       </c>
-      <c r="AI7" s="91">
+      <c r="AI7" s="61">
         <v>26</v>
       </c>
-      <c r="AJ7" s="105">
+      <c r="AJ7" s="75">
         <v>15.5</v>
       </c>
       <c r="AK7" s="21">
@@ -3061,7 +3064,7 @@
       <c r="AS7" s="21">
         <v>22</v>
       </c>
-      <c r="AT7" s="106">
+      <c r="AT7" s="76">
         <v>22</v>
       </c>
       <c r="AU7" s="56">
@@ -3164,7 +3167,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:79" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <f t="shared" si="0"/>
         <v>2500</v>
@@ -3173,7 +3176,7 @@
         <f t="shared" si="1"/>
         <v>3000</v>
       </c>
-      <c r="C8" s="116">
+      <c r="C8" s="85">
         <v>18.5</v>
       </c>
       <c r="D8" s="20">
@@ -3203,7 +3206,7 @@
       <c r="L8" s="20">
         <v>28.5</v>
       </c>
-      <c r="M8" s="117">
+      <c r="M8" s="86">
         <v>28.5</v>
       </c>
       <c r="N8" s="56">
@@ -3269,10 +3272,10 @@
       <c r="AH8" s="20">
         <v>26</v>
       </c>
-      <c r="AI8" s="91">
+      <c r="AI8" s="61">
         <v>26</v>
       </c>
-      <c r="AJ8" s="105">
+      <c r="AJ8" s="75">
         <v>15.5</v>
       </c>
       <c r="AK8" s="21">
@@ -3302,7 +3305,7 @@
       <c r="AS8" s="21">
         <v>22</v>
       </c>
-      <c r="AT8" s="106">
+      <c r="AT8" s="76">
         <v>22</v>
       </c>
       <c r="AU8" s="56">
@@ -3405,7 +3408,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:79" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:79" s="1" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <f t="shared" si="0"/>
         <v>3000</v>
@@ -3414,7 +3417,7 @@
         <f t="shared" si="1"/>
         <v>3500</v>
       </c>
-      <c r="C9" s="116">
+      <c r="C9" s="85">
         <v>18.5</v>
       </c>
       <c r="D9" s="20">
@@ -3444,7 +3447,7 @@
       <c r="L9" s="20">
         <v>30.5</v>
       </c>
-      <c r="M9" s="117">
+      <c r="M9" s="86">
         <v>30.5</v>
       </c>
       <c r="N9" s="1">
@@ -3513,37 +3516,37 @@
       <c r="AI9" s="1">
         <v>36</v>
       </c>
-      <c r="AJ9" s="107">
+      <c r="AJ9" s="77">
         <v>18</v>
       </c>
-      <c r="AK9" s="108">
+      <c r="AK9" s="1">
         <v>22</v>
       </c>
-      <c r="AL9" s="108">
+      <c r="AL9" s="1">
         <v>18</v>
       </c>
-      <c r="AM9" s="108">
+      <c r="AM9" s="1">
         <v>22</v>
       </c>
-      <c r="AN9" s="108">
+      <c r="AN9" s="1">
         <v>22</v>
       </c>
-      <c r="AO9" s="108">
+      <c r="AO9" s="1">
         <v>22</v>
       </c>
-      <c r="AP9" s="108">
+      <c r="AP9" s="1">
         <v>22</v>
       </c>
-      <c r="AQ9" s="108">
+      <c r="AQ9" s="1">
         <v>22</v>
       </c>
-      <c r="AR9" s="108">
+      <c r="AR9" s="1">
         <v>22</v>
       </c>
-      <c r="AS9" s="108">
+      <c r="AS9" s="1">
         <v>22</v>
       </c>
-      <c r="AT9" s="109">
+      <c r="AT9" s="78">
         <v>22</v>
       </c>
       <c r="AU9" s="1">
@@ -3646,7 +3649,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:79" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <f t="shared" si="0"/>
         <v>3500</v>
@@ -3655,7 +3658,7 @@
         <f t="shared" si="1"/>
         <v>4000</v>
       </c>
-      <c r="C10" s="116">
+      <c r="C10" s="85">
         <v>18.5</v>
       </c>
       <c r="D10" s="20">
@@ -3685,7 +3688,7 @@
       <c r="L10" s="20">
         <v>30.5</v>
       </c>
-      <c r="M10" s="117">
+      <c r="M10" s="86">
         <v>30.5</v>
       </c>
       <c r="N10" s="56">
@@ -3751,10 +3754,10 @@
       <c r="AH10" s="20">
         <v>36</v>
       </c>
-      <c r="AI10" s="91">
+      <c r="AI10" s="61">
         <v>36</v>
       </c>
-      <c r="AJ10" s="105">
+      <c r="AJ10" s="75">
         <v>20.5</v>
       </c>
       <c r="AK10" s="21">
@@ -3784,7 +3787,7 @@
       <c r="AS10" s="21">
         <v>22</v>
       </c>
-      <c r="AT10" s="106">
+      <c r="AT10" s="76">
         <v>22</v>
       </c>
       <c r="AU10" s="56">
@@ -3887,7 +3890,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:79" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <f t="shared" si="0"/>
         <v>4000</v>
@@ -3896,7 +3899,7 @@
         <f t="shared" si="1"/>
         <v>4500</v>
       </c>
-      <c r="C11" s="116">
+      <c r="C11" s="85">
         <v>18.5</v>
       </c>
       <c r="D11" s="20">
@@ -3926,7 +3929,7 @@
       <c r="L11" s="20">
         <v>33.5</v>
       </c>
-      <c r="M11" s="117">
+      <c r="M11" s="86">
         <v>33.5</v>
       </c>
       <c r="N11" s="56">
@@ -3992,10 +3995,10 @@
       <c r="AH11" s="20">
         <v>46</v>
       </c>
-      <c r="AI11" s="91">
+      <c r="AI11" s="61">
         <v>46</v>
       </c>
-      <c r="AJ11" s="105">
+      <c r="AJ11" s="75">
         <v>22</v>
       </c>
       <c r="AK11" s="21">
@@ -4025,7 +4028,7 @@
       <c r="AS11" s="21">
         <v>22</v>
       </c>
-      <c r="AT11" s="106">
+      <c r="AT11" s="76">
         <v>22</v>
       </c>
       <c r="AU11" s="56">
@@ -4128,7 +4131,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:79" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <f t="shared" si="0"/>
         <v>4500</v>
@@ -4137,7 +4140,7 @@
         <f t="shared" si="1"/>
         <v>5000</v>
       </c>
-      <c r="C12" s="116">
+      <c r="C12" s="85">
         <v>18.5</v>
       </c>
       <c r="D12" s="20">
@@ -4167,7 +4170,7 @@
       <c r="L12" s="20">
         <v>33.5</v>
       </c>
-      <c r="M12" s="117">
+      <c r="M12" s="86">
         <v>33.5</v>
       </c>
       <c r="N12" s="56">
@@ -4233,10 +4236,10 @@
       <c r="AH12" s="20">
         <v>46</v>
       </c>
-      <c r="AI12" s="91">
+      <c r="AI12" s="61">
         <v>46</v>
       </c>
-      <c r="AJ12" s="105">
+      <c r="AJ12" s="75">
         <v>22</v>
       </c>
       <c r="AK12" s="21">
@@ -4266,7 +4269,7 @@
       <c r="AS12" s="21">
         <v>22</v>
       </c>
-      <c r="AT12" s="106">
+      <c r="AT12" s="76">
         <v>22</v>
       </c>
       <c r="AU12" s="56">
@@ -4369,7 +4372,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:79" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <f t="shared" si="0"/>
         <v>5000</v>
@@ -4378,7 +4381,7 @@
         <f t="shared" si="1"/>
         <v>5500</v>
       </c>
-      <c r="C13" s="116">
+      <c r="C13" s="85">
         <v>26.5</v>
       </c>
       <c r="D13" s="20">
@@ -4408,7 +4411,7 @@
       <c r="L13" s="20">
         <v>43.5</v>
       </c>
-      <c r="M13" s="117">
+      <c r="M13" s="86">
         <v>39.5</v>
       </c>
       <c r="N13" s="56">
@@ -4474,10 +4477,10 @@
       <c r="AH13" s="20">
         <v>56</v>
       </c>
-      <c r="AI13" s="91">
+      <c r="AI13" s="61">
         <v>56</v>
       </c>
-      <c r="AJ13" s="105">
+      <c r="AJ13" s="75">
         <v>26</v>
       </c>
       <c r="AK13" s="21">
@@ -4507,7 +4510,7 @@
       <c r="AS13" s="21">
         <v>29</v>
       </c>
-      <c r="AT13" s="106">
+      <c r="AT13" s="76">
         <v>29</v>
       </c>
       <c r="AU13" s="56">
@@ -4610,7 +4613,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:79" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <f t="shared" si="0"/>
         <v>5500</v>
@@ -4619,7 +4622,7 @@
         <f t="shared" si="1"/>
         <v>6000</v>
       </c>
-      <c r="C14" s="116">
+      <c r="C14" s="85">
         <v>26.5</v>
       </c>
       <c r="D14" s="20">
@@ -4649,7 +4652,7 @@
       <c r="L14" s="20">
         <v>43.5</v>
       </c>
-      <c r="M14" s="117">
+      <c r="M14" s="86">
         <v>39.5</v>
       </c>
       <c r="N14" s="56">
@@ -4715,10 +4718,10 @@
       <c r="AH14" s="20">
         <v>56</v>
       </c>
-      <c r="AI14" s="91">
+      <c r="AI14" s="61">
         <v>56</v>
       </c>
-      <c r="AJ14" s="105">
+      <c r="AJ14" s="75">
         <v>30</v>
       </c>
       <c r="AK14" s="21">
@@ -4748,7 +4751,7 @@
       <c r="AS14" s="21">
         <v>35</v>
       </c>
-      <c r="AT14" s="106">
+      <c r="AT14" s="76">
         <v>35</v>
       </c>
       <c r="AU14" s="56">
@@ -4851,7 +4854,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:79" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <f t="shared" si="0"/>
         <v>6000</v>
@@ -4860,7 +4863,7 @@
         <f t="shared" si="1"/>
         <v>6500</v>
       </c>
-      <c r="C15" s="116">
+      <c r="C15" s="85">
         <v>26.5</v>
       </c>
       <c r="D15" s="20">
@@ -4890,7 +4893,7 @@
       <c r="L15" s="20">
         <v>43.5</v>
       </c>
-      <c r="M15" s="117">
+      <c r="M15" s="86">
         <v>39.5</v>
       </c>
       <c r="N15" s="56">
@@ -4956,10 +4959,10 @@
       <c r="AH15" s="20">
         <v>66</v>
       </c>
-      <c r="AI15" s="91">
+      <c r="AI15" s="61">
         <v>66</v>
       </c>
-      <c r="AJ15" s="105">
+      <c r="AJ15" s="75">
         <v>34</v>
       </c>
       <c r="AK15" s="21">
@@ -4989,7 +4992,7 @@
       <c r="AS15" s="21">
         <v>41</v>
       </c>
-      <c r="AT15" s="106">
+      <c r="AT15" s="76">
         <v>41</v>
       </c>
       <c r="AU15" s="56">
@@ -5092,7 +5095,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:79" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <f t="shared" si="0"/>
         <v>6500</v>
@@ -5101,7 +5104,7 @@
         <f>B15+500</f>
         <v>7000</v>
       </c>
-      <c r="C16" s="116">
+      <c r="C16" s="85">
         <v>26.5</v>
       </c>
       <c r="D16" s="20">
@@ -5131,7 +5134,7 @@
       <c r="L16" s="20">
         <v>43.5</v>
       </c>
-      <c r="M16" s="117">
+      <c r="M16" s="86">
         <v>39.5</v>
       </c>
       <c r="N16" s="56">
@@ -5197,10 +5200,10 @@
       <c r="AH16" s="20">
         <v>66</v>
       </c>
-      <c r="AI16" s="91">
+      <c r="AI16" s="61">
         <v>66</v>
       </c>
-      <c r="AJ16" s="105">
+      <c r="AJ16" s="75">
         <v>38</v>
       </c>
       <c r="AK16" s="21">
@@ -5230,7 +5233,7 @@
       <c r="AS16" s="21">
         <v>41</v>
       </c>
-      <c r="AT16" s="106">
+      <c r="AT16" s="76">
         <v>41</v>
       </c>
       <c r="AU16" s="56">
@@ -5333,7 +5336,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:79" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <f t="shared" si="0"/>
         <v>7000</v>
@@ -5342,7 +5345,7 @@
         <f t="shared" si="1"/>
         <v>7500</v>
       </c>
-      <c r="C17" s="116">
+      <c r="C17" s="85">
         <v>36.5</v>
       </c>
       <c r="D17" s="20">
@@ -5372,7 +5375,7 @@
       <c r="L17" s="20">
         <v>60.5</v>
       </c>
-      <c r="M17" s="117">
+      <c r="M17" s="86">
         <v>58.5</v>
       </c>
       <c r="N17" s="56">
@@ -5438,10 +5441,10 @@
       <c r="AH17" s="20">
         <v>76</v>
       </c>
-      <c r="AI17" s="91">
+      <c r="AI17" s="61">
         <v>76</v>
       </c>
-      <c r="AJ17" s="105">
+      <c r="AJ17" s="75">
         <v>43</v>
       </c>
       <c r="AK17" s="21">
@@ -5471,7 +5474,7 @@
       <c r="AS17" s="21">
         <v>47</v>
       </c>
-      <c r="AT17" s="106">
+      <c r="AT17" s="76">
         <v>47</v>
       </c>
       <c r="AU17" s="56">
@@ -5574,7 +5577,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:79" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <f t="shared" si="0"/>
         <v>7500</v>
@@ -5583,7 +5586,7 @@
         <f t="shared" si="1"/>
         <v>8000</v>
       </c>
-      <c r="C18" s="116">
+      <c r="C18" s="85">
         <v>36.5</v>
       </c>
       <c r="D18" s="20">
@@ -5613,7 +5616,7 @@
       <c r="L18" s="20">
         <v>60.5</v>
       </c>
-      <c r="M18" s="117">
+      <c r="M18" s="86">
         <v>58.5</v>
       </c>
       <c r="N18" s="56">
@@ -5679,10 +5682,10 @@
       <c r="AH18" s="20">
         <v>76</v>
       </c>
-      <c r="AI18" s="91">
+      <c r="AI18" s="61">
         <v>76</v>
       </c>
-      <c r="AJ18" s="105">
+      <c r="AJ18" s="75">
         <v>46</v>
       </c>
       <c r="AK18" s="21">
@@ -5712,7 +5715,7 @@
       <c r="AS18" s="21">
         <v>47</v>
       </c>
-      <c r="AT18" s="106">
+      <c r="AT18" s="76">
         <v>47</v>
       </c>
       <c r="AU18" s="56">
@@ -5815,7 +5818,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="19" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:79" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <f t="shared" si="0"/>
         <v>8000</v>
@@ -5824,7 +5827,7 @@
         <f t="shared" si="1"/>
         <v>8500</v>
       </c>
-      <c r="C19" s="116">
+      <c r="C19" s="85">
         <v>36.5</v>
       </c>
       <c r="D19" s="20">
@@ -5854,7 +5857,7 @@
       <c r="L19" s="20">
         <v>60.5</v>
       </c>
-      <c r="M19" s="117">
+      <c r="M19" s="86">
         <v>58.5</v>
       </c>
       <c r="N19" s="56">
@@ -5920,10 +5923,10 @@
       <c r="AH19" s="20">
         <v>86</v>
       </c>
-      <c r="AI19" s="91">
+      <c r="AI19" s="61">
         <v>86</v>
       </c>
-      <c r="AJ19" s="105">
+      <c r="AJ19" s="75">
         <v>49</v>
       </c>
       <c r="AK19" s="21">
@@ -5953,7 +5956,7 @@
       <c r="AS19" s="21">
         <v>49</v>
       </c>
-      <c r="AT19" s="106">
+      <c r="AT19" s="76">
         <v>49</v>
       </c>
       <c r="AU19" s="56">
@@ -6056,7 +6059,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:79" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <f t="shared" si="0"/>
         <v>8500</v>
@@ -6065,7 +6068,7 @@
         <f>B19+500</f>
         <v>9000</v>
       </c>
-      <c r="C20" s="116">
+      <c r="C20" s="85">
         <v>36.5</v>
       </c>
       <c r="D20" s="20">
@@ -6095,7 +6098,7 @@
       <c r="L20" s="20">
         <v>60.5</v>
       </c>
-      <c r="M20" s="117">
+      <c r="M20" s="86">
         <v>58.5</v>
       </c>
       <c r="N20" s="56">
@@ -6161,10 +6164,10 @@
       <c r="AH20" s="20">
         <v>86</v>
       </c>
-      <c r="AI20" s="91">
+      <c r="AI20" s="61">
         <v>86</v>
       </c>
-      <c r="AJ20" s="105">
+      <c r="AJ20" s="75">
         <v>49</v>
       </c>
       <c r="AK20" s="21">
@@ -6194,7 +6197,7 @@
       <c r="AS20" s="21">
         <v>49</v>
       </c>
-      <c r="AT20" s="106">
+      <c r="AT20" s="76">
         <v>49</v>
       </c>
       <c r="AU20" s="56">
@@ -6297,7 +6300,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="21" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:79" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <f t="shared" si="0"/>
         <v>9000</v>
@@ -6306,7 +6309,7 @@
         <f t="shared" si="1"/>
         <v>9500</v>
       </c>
-      <c r="C21" s="116">
+      <c r="C21" s="85">
         <v>36.5</v>
       </c>
       <c r="D21" s="20">
@@ -6336,7 +6339,7 @@
       <c r="L21" s="20">
         <v>60.5</v>
       </c>
-      <c r="M21" s="117">
+      <c r="M21" s="86">
         <v>58.5</v>
       </c>
       <c r="N21" s="56">
@@ -6402,10 +6405,10 @@
       <c r="AH21" s="20">
         <v>96</v>
       </c>
-      <c r="AI21" s="91">
+      <c r="AI21" s="61">
         <v>96</v>
       </c>
-      <c r="AJ21" s="105">
+      <c r="AJ21" s="75">
         <v>49</v>
       </c>
       <c r="AK21" s="21">
@@ -6435,7 +6438,7 @@
       <c r="AS21" s="21">
         <v>49</v>
       </c>
-      <c r="AT21" s="106">
+      <c r="AT21" s="76">
         <v>49</v>
       </c>
       <c r="AU21" s="56">
@@ -6538,47 +6541,47 @@
         <v>49</v>
       </c>
     </row>
-    <row r="22" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:79" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>9500</v>
       </c>
       <c r="B22" s="5">
         <v>10000</v>
       </c>
-      <c r="C22" s="118">
+      <c r="C22" s="87">
         <v>36.5</v>
       </c>
-      <c r="D22" s="119">
+      <c r="D22" s="88">
         <v>36.5</v>
       </c>
-      <c r="E22" s="119">
+      <c r="E22" s="88">
         <v>36.5</v>
       </c>
-      <c r="F22" s="119">
+      <c r="F22" s="88">
         <v>36.5</v>
       </c>
-      <c r="G22" s="119">
+      <c r="G22" s="88">
         <v>38.5</v>
       </c>
-      <c r="H22" s="119">
+      <c r="H22" s="88">
         <v>60.5</v>
       </c>
-      <c r="I22" s="119">
+      <c r="I22" s="88">
         <v>60.5</v>
       </c>
-      <c r="J22" s="119">
+      <c r="J22" s="88">
         <v>38.5</v>
       </c>
-      <c r="K22" s="119">
+      <c r="K22" s="88">
         <v>60.5</v>
       </c>
-      <c r="L22" s="119">
+      <c r="L22" s="88">
         <v>60.5</v>
       </c>
-      <c r="M22" s="120">
+      <c r="M22" s="89">
         <v>58.5</v>
       </c>
-      <c r="N22" s="97">
+      <c r="N22" s="67">
         <v>37</v>
       </c>
       <c r="O22" s="41">
@@ -6641,43 +6644,43 @@
       <c r="AH22" s="28">
         <v>96</v>
       </c>
-      <c r="AI22" s="92">
+      <c r="AI22" s="62">
         <v>96</v>
       </c>
-      <c r="AJ22" s="110">
+      <c r="AJ22" s="79">
         <v>49</v>
       </c>
-      <c r="AK22" s="111">
+      <c r="AK22" s="80">
         <v>49</v>
       </c>
-      <c r="AL22" s="111">
+      <c r="AL22" s="80">
         <v>49</v>
       </c>
-      <c r="AM22" s="111">
+      <c r="AM22" s="80">
         <v>49</v>
       </c>
-      <c r="AN22" s="111">
+      <c r="AN22" s="80">
         <v>49</v>
       </c>
-      <c r="AO22" s="111">
+      <c r="AO22" s="80">
         <v>49</v>
       </c>
-      <c r="AP22" s="111">
+      <c r="AP22" s="80">
         <v>49</v>
       </c>
-      <c r="AQ22" s="111">
+      <c r="AQ22" s="80">
         <v>49</v>
       </c>
-      <c r="AR22" s="111">
+      <c r="AR22" s="80">
         <v>49</v>
       </c>
-      <c r="AS22" s="111">
+      <c r="AS22" s="80">
         <v>49</v>
       </c>
-      <c r="AT22" s="112">
+      <c r="AT22" s="81">
         <v>49</v>
       </c>
-      <c r="AU22" s="97">
+      <c r="AU22" s="67">
         <v>46</v>
       </c>
       <c r="AV22" s="41">
@@ -6777,7 +6780,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="23" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
         <f>A22+500</f>
         <v>10000</v>
@@ -6831,7 +6834,7 @@
         <v>73.5</v>
       </c>
       <c r="N23" s="32">
-        <f t="shared" ref="D23:N23" si="3">N22+N$103</f>
+        <f t="shared" ref="N23" si="3">N22+N$103</f>
         <v>39</v>
       </c>
       <c r="O23" s="33">
@@ -7095,7 +7098,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="24" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
         <f t="shared" ref="A24:A26" si="36">A23+500</f>
         <v>10500</v>
@@ -7413,7 +7416,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
         <f t="shared" si="36"/>
         <v>11000</v>
@@ -7731,7 +7734,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="26" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
         <f t="shared" si="36"/>
         <v>11500</v>
@@ -8049,7 +8052,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="27" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A27" s="3">
         <f t="shared" ref="A27:A46" si="71">A26+500</f>
         <v>12000</v>
@@ -8367,7 +8370,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="28" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A28" s="3">
         <f t="shared" si="71"/>
         <v>12500</v>
@@ -8685,7 +8688,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="29" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A29" s="3">
         <f t="shared" si="71"/>
         <v>13000</v>
@@ -9003,7 +9006,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="30" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A30" s="3">
         <f t="shared" si="71"/>
         <v>13500</v>
@@ -9321,7 +9324,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="31" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A31" s="3">
         <f t="shared" si="71"/>
         <v>14000</v>
@@ -9639,7 +9642,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="32" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A32" s="3">
         <f t="shared" si="71"/>
         <v>14500</v>
@@ -9957,7 +9960,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="33" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A33" s="3">
         <f t="shared" si="71"/>
         <v>15000</v>
@@ -10275,7 +10278,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="34" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A34" s="3">
         <f t="shared" si="71"/>
         <v>15500</v>
@@ -10593,7 +10596,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="35" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A35" s="3">
         <f t="shared" si="71"/>
         <v>16000</v>
@@ -10911,7 +10914,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="36" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A36" s="3">
         <f t="shared" si="71"/>
         <v>16500</v>
@@ -11229,7 +11232,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="37" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A37" s="3">
         <f t="shared" si="71"/>
         <v>17000</v>
@@ -11547,7 +11550,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="38" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A38" s="3">
         <f t="shared" si="71"/>
         <v>17500</v>
@@ -11865,7 +11868,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="39" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A39" s="3">
         <f t="shared" si="71"/>
         <v>18000</v>
@@ -12183,7 +12186,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="40" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A40" s="3">
         <f t="shared" si="71"/>
         <v>18500</v>
@@ -12501,7 +12504,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="41" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A41" s="3">
         <f t="shared" si="71"/>
         <v>19000</v>
@@ -12819,7 +12822,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="42" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A42" s="3">
         <f t="shared" si="71"/>
         <v>19500</v>
@@ -13137,7 +13140,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="43" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A43" s="3">
         <f t="shared" si="71"/>
         <v>20000</v>
@@ -13455,7 +13458,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="44" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A44" s="3">
         <f t="shared" si="71"/>
         <v>20500</v>
@@ -13773,7 +13776,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="45" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A45" s="3">
         <f t="shared" si="71"/>
         <v>21000</v>
@@ -14091,7 +14094,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="46" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A46" s="3">
         <f t="shared" si="71"/>
         <v>21500</v>
@@ -14409,7 +14412,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="47" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A47" s="3">
         <f>A46+500</f>
         <v>22000</v>
@@ -14727,7 +14730,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="48" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A48" s="3">
         <f t="shared" ref="A48:A58" si="79">A47+500</f>
         <v>22500</v>
@@ -15045,7 +15048,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="49" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A49" s="3">
         <f t="shared" si="79"/>
         <v>23000</v>
@@ -15363,7 +15366,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="50" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A50" s="3">
         <f t="shared" si="79"/>
         <v>23500</v>
@@ -15681,7 +15684,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="51" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A51" s="3">
         <f t="shared" si="79"/>
         <v>24000</v>
@@ -15999,7 +16002,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="52" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A52" s="3">
         <f t="shared" si="79"/>
         <v>24500</v>
@@ -16317,7 +16320,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="53" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A53" s="3">
         <f t="shared" si="79"/>
         <v>25000</v>
@@ -16635,7 +16638,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="54" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A54" s="3">
         <f t="shared" si="79"/>
         <v>25500</v>
@@ -16953,7 +16956,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="55" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A55" s="3">
         <f t="shared" si="79"/>
         <v>26000</v>
@@ -17271,7 +17274,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="56" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A56" s="3">
         <f t="shared" si="79"/>
         <v>26500</v>
@@ -17281,7 +17284,7 @@
         <v>27000</v>
       </c>
       <c r="C56" s="36">
-        <f t="shared" ref="C56:M102" si="81">C$22 + C$103*CEILING($B56-$A$23,1000)/1000</f>
+        <f t="shared" ref="C56:M79" si="81">C$22 + C$103*CEILING($B56-$A$23,1000)/1000</f>
         <v>223.5</v>
       </c>
       <c r="D56" s="36">
@@ -17589,7 +17592,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="57" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A57" s="3">
         <f t="shared" si="79"/>
         <v>27000</v>
@@ -17907,7 +17910,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="58" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A58" s="3">
         <f t="shared" si="79"/>
         <v>27500</v>
@@ -18225,7 +18228,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="59" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A59" s="3">
         <f>A58+500</f>
         <v>28000</v>
@@ -18543,7 +18546,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="60" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A60" s="3">
         <f t="shared" ref="A60:A102" si="82">A59+500</f>
         <v>28500</v>
@@ -18861,7 +18864,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="61" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A61" s="3">
         <f t="shared" si="82"/>
         <v>29000</v>
@@ -19179,7 +19182,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="62" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A62" s="3">
         <f t="shared" si="82"/>
         <v>29500</v>
@@ -19497,7 +19500,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="63" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A63" s="3">
         <f t="shared" si="82"/>
         <v>30000</v>
@@ -19815,7 +19818,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="64" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A64" s="3">
         <f t="shared" si="82"/>
         <v>30500</v>
@@ -20133,7 +20136,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="65" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A65" s="3">
         <f t="shared" si="82"/>
         <v>31000</v>
@@ -20451,7 +20454,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="66" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A66" s="3">
         <f t="shared" si="82"/>
         <v>31500</v>
@@ -20769,7 +20772,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="67" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A67" s="3">
         <f t="shared" si="82"/>
         <v>32000</v>
@@ -21087,7 +21090,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="68" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A68" s="3">
         <f t="shared" si="82"/>
         <v>32500</v>
@@ -21405,7 +21408,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="69" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A69" s="3">
         <f t="shared" si="82"/>
         <v>33000</v>
@@ -21723,7 +21726,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="70" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A70" s="3">
         <f t="shared" si="82"/>
         <v>33500</v>
@@ -22041,7 +22044,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="71" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A71" s="3">
         <f t="shared" si="82"/>
         <v>34000</v>
@@ -22359,7 +22362,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="72" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A72" s="3">
         <f t="shared" si="82"/>
         <v>34500</v>
@@ -22677,7 +22680,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="73" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A73" s="3">
         <f t="shared" si="82"/>
         <v>35000</v>
@@ -22995,7 +22998,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="74" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A74" s="3">
         <f t="shared" si="82"/>
         <v>35500</v>
@@ -23313,7 +23316,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="75" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A75" s="3">
         <f t="shared" si="82"/>
         <v>36000</v>
@@ -23631,7 +23634,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="76" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A76" s="3">
         <f t="shared" si="82"/>
         <v>36500</v>
@@ -23949,7 +23952,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="77" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A77" s="3">
         <f t="shared" si="82"/>
         <v>37000</v>
@@ -24267,7 +24270,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="78" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A78" s="3">
         <f t="shared" si="82"/>
         <v>37500</v>
@@ -24585,7 +24588,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="79" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A79" s="3">
         <f t="shared" si="82"/>
         <v>38000</v>
@@ -24903,7 +24906,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="80" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A80" s="3">
         <f t="shared" si="82"/>
         <v>38500</v>
@@ -25221,7 +25224,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="81" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A81" s="3">
         <f t="shared" si="82"/>
         <v>39000</v>
@@ -25539,7 +25542,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="82" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A82" s="3">
         <f t="shared" si="82"/>
         <v>39500</v>
@@ -25857,7 +25860,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="83" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A83" s="3">
         <f t="shared" si="82"/>
         <v>40000</v>
@@ -26175,7 +26178,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="84" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A84" s="3">
         <f t="shared" si="82"/>
         <v>40500</v>
@@ -26493,7 +26496,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="85" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A85" s="3">
         <f t="shared" si="82"/>
         <v>41000</v>
@@ -26811,7 +26814,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="86" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A86" s="3">
         <f t="shared" si="82"/>
         <v>41500</v>
@@ -27129,7 +27132,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="87" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A87" s="3">
         <f t="shared" si="82"/>
         <v>42000</v>
@@ -27447,7 +27450,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="88" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A88" s="3">
         <f t="shared" si="82"/>
         <v>42500</v>
@@ -27765,7 +27768,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="89" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A89" s="3">
         <f t="shared" si="82"/>
         <v>43000</v>
@@ -28083,7 +28086,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="90" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A90" s="3">
         <f t="shared" si="82"/>
         <v>43500</v>
@@ -28401,7 +28404,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="91" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A91" s="3">
         <f t="shared" si="82"/>
         <v>44000</v>
@@ -28719,7 +28722,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="92" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A92" s="3">
         <f t="shared" si="82"/>
         <v>44500</v>
@@ -29037,7 +29040,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="93" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A93" s="3">
         <f t="shared" si="82"/>
         <v>45000</v>
@@ -29355,7 +29358,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="94" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A94" s="3">
         <f t="shared" si="82"/>
         <v>45500</v>
@@ -29673,7 +29676,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="95" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A95" s="3">
         <f t="shared" si="82"/>
         <v>46000</v>
@@ -29991,7 +29994,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="96" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A96" s="3">
         <f t="shared" si="82"/>
         <v>46500</v>
@@ -30309,7 +30312,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="97" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A97" s="3">
         <f t="shared" si="82"/>
         <v>47000</v>
@@ -30627,7 +30630,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="98" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A98" s="3">
         <f t="shared" si="82"/>
         <v>47500</v>
@@ -30945,7 +30948,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="99" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A99" s="3">
         <f t="shared" si="82"/>
         <v>48000</v>
@@ -31263,7 +31266,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="100" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A100" s="3">
         <f t="shared" si="82"/>
         <v>48500</v>
@@ -31581,7 +31584,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="101" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A101" s="3">
         <f t="shared" si="82"/>
         <v>49000</v>
@@ -31899,7 +31902,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="102" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:79" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A102" s="3">
         <f t="shared" si="82"/>
         <v>49500</v>
@@ -32217,11 +32220,11 @@
         <v>249</v>
       </c>
     </row>
-    <row r="103" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A103" s="61" t="s">
+    <row r="103" spans="1:79" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A103" s="97" t="s">
         <v>12</v>
       </c>
-      <c r="B103" s="62"/>
+      <c r="B103" s="98"/>
       <c r="C103" s="29">
         <v>11</v>
       </c>
@@ -32454,11 +32457,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="104" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A104" s="63" t="s">
+    <row r="104" spans="1:79" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A104" s="99" t="s">
         <v>13</v>
       </c>
-      <c r="B104" s="64"/>
+      <c r="B104" s="100"/>
       <c r="C104" s="23">
         <v>11</v>
       </c>
@@ -32691,11 +32694,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="105" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A105" s="65" t="s">
+    <row r="105" spans="1:79" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A105" s="101" t="s">
         <v>20</v>
       </c>
-      <c r="B105" s="66"/>
+      <c r="B105" s="102"/>
       <c r="C105" s="2"/>
       <c r="D105" s="2"/>
       <c r="E105" s="2"/>
@@ -32740,243 +32743,238 @@
       <c r="AR105" s="9"/>
       <c r="AS105" s="9"/>
       <c r="AT105" s="9"/>
-      <c r="AU105" s="67" t="s">
+      <c r="AU105" s="103" t="s">
         <v>18</v>
       </c>
-      <c r="AV105" s="68"/>
-      <c r="AW105" s="68"/>
-      <c r="AX105" s="69"/>
-      <c r="AY105" s="70" t="s">
+      <c r="AV105" s="104"/>
+      <c r="AW105" s="104"/>
+      <c r="AX105" s="105"/>
+      <c r="AY105" s="106" t="s">
         <v>19</v>
       </c>
-      <c r="AZ105" s="71"/>
-      <c r="BA105" s="71"/>
-      <c r="BB105" s="71"/>
-      <c r="BC105" s="71"/>
-      <c r="BD105" s="71"/>
-      <c r="BE105" s="71"/>
-      <c r="BF105" s="72"/>
-      <c r="BG105" s="73"/>
-      <c r="BH105" s="73"/>
-      <c r="BI105" s="73"/>
-      <c r="BJ105" s="73"/>
-      <c r="BK105" s="73"/>
-      <c r="BL105" s="73"/>
-      <c r="BM105" s="73"/>
-      <c r="BN105" s="73"/>
-      <c r="BO105" s="73"/>
-      <c r="BP105" s="74"/>
-      <c r="BQ105" s="72"/>
-      <c r="BR105" s="73"/>
-      <c r="BS105" s="73"/>
-      <c r="BT105" s="73"/>
-      <c r="BU105" s="73"/>
-      <c r="BV105" s="73"/>
-      <c r="BW105" s="73"/>
-      <c r="BX105" s="73"/>
-      <c r="BY105" s="73"/>
-      <c r="BZ105" s="73"/>
-      <c r="CA105" s="74"/>
+      <c r="AZ105" s="107"/>
+      <c r="BA105" s="107"/>
+      <c r="BB105" s="107"/>
+      <c r="BC105" s="107"/>
+      <c r="BD105" s="107"/>
+      <c r="BE105" s="107"/>
+      <c r="BF105" s="92"/>
+      <c r="BG105" s="93"/>
+      <c r="BH105" s="93"/>
+      <c r="BI105" s="93"/>
+      <c r="BJ105" s="93"/>
+      <c r="BK105" s="93"/>
+      <c r="BL105" s="93"/>
+      <c r="BM105" s="93"/>
+      <c r="BN105" s="93"/>
+      <c r="BO105" s="93"/>
+      <c r="BP105" s="94"/>
+      <c r="BQ105" s="92"/>
+      <c r="BR105" s="93"/>
+      <c r="BS105" s="93"/>
+      <c r="BT105" s="93"/>
+      <c r="BU105" s="93"/>
+      <c r="BV105" s="93"/>
+      <c r="BW105" s="93"/>
+      <c r="BX105" s="93"/>
+      <c r="BY105" s="93"/>
+      <c r="BZ105" s="93"/>
+      <c r="CA105" s="94"/>
     </row>
-    <row r="106" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A106" s="3"/>
     </row>
-    <row r="107" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A107" s="3"/>
     </row>
-    <row r="108" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A108" s="3"/>
     </row>
-    <row r="109" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A109" s="3"/>
     </row>
-    <row r="110" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A110" s="3"/>
     </row>
-    <row r="111" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A111" s="3"/>
     </row>
-    <row r="112" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A112" s="3"/>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A113" s="3"/>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A114" s="3"/>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A115" s="3"/>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A116" s="3"/>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A117" s="3"/>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A118" s="3"/>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A119" s="3"/>
     </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A120" s="3"/>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A121" s="3"/>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A122" s="3"/>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A123" s="3"/>
     </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A124" s="3"/>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A125" s="3"/>
     </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A126" s="3"/>
     </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A127" s="3"/>
     </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A128" s="3"/>
     </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A129" s="3"/>
     </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A130" s="3"/>
     </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A131" s="3"/>
     </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A132" s="3"/>
     </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A133" s="3"/>
     </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A134" s="3"/>
     </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A135" s="3"/>
     </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A136" s="3"/>
     </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A137" s="3"/>
     </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A138" s="3"/>
     </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A139" s="3"/>
     </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A140" s="3"/>
     </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A141" s="3"/>
     </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A142" s="3"/>
     </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A143" s="3"/>
     </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A144" s="3"/>
     </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A145" s="3"/>
     </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A146" s="3"/>
     </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A147" s="3"/>
     </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A148" s="3"/>
     </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A149" s="3"/>
     </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A150" s="3"/>
     </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A151" s="3"/>
     </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A152" s="3"/>
     </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A153" s="3"/>
     </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A154" s="3"/>
     </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A155" s="3"/>
     </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A156" s="3"/>
     </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A157" s="3"/>
     </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A158" s="3"/>
     </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A159" s="3"/>
     </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A160" s="3"/>
     </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A161" s="3"/>
     </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A162" s="3"/>
     </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A163" s="3"/>
     </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A164" s="3"/>
     </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A165" s="3"/>
     </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A166" s="3"/>
     </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A167" s="3"/>
     </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A168" s="3"/>
     </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A169" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="AJ1:AT1"/>
-    <mergeCell ref="Y1:AI1"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="N1:X1"/>
-    <mergeCell ref="C1:M1"/>
     <mergeCell ref="BF105:BP105"/>
     <mergeCell ref="BQ105:CA105"/>
     <mergeCell ref="BQ1:CA1"/>
@@ -32986,6 +32984,11 @@
     <mergeCell ref="A105:B105"/>
     <mergeCell ref="AU105:AX105"/>
     <mergeCell ref="AY105:BE105"/>
+    <mergeCell ref="AJ1:AT1"/>
+    <mergeCell ref="Y1:AI1"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="N1:X1"/>
+    <mergeCell ref="C1:M1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>